<commit_message>
refining text and analyses
</commit_message>
<xml_diff>
--- a/data/data_gridsearch_subjects.xlsx
+++ b/data/data_gridsearch_subjects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hmupm-my.sharepoint.com/personal/bjoern_meder_hmu-potsdam_de/Documents/_Projekte/gridsearch Parkinson/2024 gridSearch Parkinson/06_github_repo/gridsearch_parkinsons/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{30E631F0-5369-664A-9279-3B69550168D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60D35704-7D62-0940-84E9-64CF2D916D05}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{30E631F0-5369-664A-9279-3B69550168D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF554B20-AAFB-DE41-AF28-879E13E9BD24}"/>
   <bookViews>
-    <workbookView xWindow="31940" yWindow="-4240" windowWidth="60160" windowHeight="33340" activeTab="2" xr2:uid="{9551D2BD-E314-0446-B93E-CE842B5EA9E5}"/>
+    <workbookView xWindow="30240" yWindow="-4540" windowWidth="60160" windowHeight="33340" activeTab="2" xr2:uid="{9551D2BD-E314-0446-B93E-CE842B5EA9E5}"/>
   </bookViews>
   <sheets>
     <sheet name="batch1" sheetId="2" r:id="rId1"/>
@@ -3364,8 +3364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD691BDA-9D3A-9C46-B4FA-85EF79BE6CF0}">
   <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="H65" sqref="H65"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5518,9 +5518,6 @@
       <c r="F76">
         <v>28</v>
       </c>
-      <c r="G76">
-        <v>2</v>
-      </c>
       <c r="J76" s="7">
         <v>0.60416666666666663</v>
       </c>

</xml_diff>

<commit_message>
started working on analyzing batch 2
</commit_message>
<xml_diff>
--- a/data/data_gridsearch_subjects.xlsx
+++ b/data/data_gridsearch_subjects.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hmupm-my.sharepoint.com/personal/bjoern_meder_hmu-potsdam_de/Documents/_Projekte/gridsearch Parkinson/2024 gridSearch Parkinson/06_github_repo/gridsearch_parkinsons/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{30E631F0-5369-664A-9279-3B69550168D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF554B20-AAFB-DE41-AF28-879E13E9BD24}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{30E631F0-5369-664A-9279-3B69550168D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5D55E68-0D97-524A-9E8C-7ADA535822E6}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="-4540" windowWidth="60160" windowHeight="33340" activeTab="2" xr2:uid="{9551D2BD-E314-0446-B93E-CE842B5EA9E5}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{9551D2BD-E314-0446-B93E-CE842B5EA9E5}"/>
   </bookViews>
   <sheets>
     <sheet name="batch1" sheetId="2" r:id="rId1"/>
     <sheet name="batch2" sheetId="1" r:id="rId2"/>
-    <sheet name="all" sheetId="3" r:id="rId3"/>
+    <sheet name="batch3" sheetId="4" r:id="rId3"/>
+    <sheet name="all" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="gridsearch_subject_data" localSheetId="2">all!$A$1:$J$63</definedName>
+    <definedName name="gridsearch_subject_data" localSheetId="3">all!$A$1:$J$63</definedName>
     <definedName name="gridsearch_subject_data" localSheetId="0">batch1!$A$1:$J$63</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -79,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="20">
   <si>
     <t>id</t>
   </si>
@@ -131,12 +132,21 @@
   <si>
     <t>w</t>
   </si>
+  <si>
+    <t>PPD</t>
+  </si>
+  <si>
+    <t>PPD+</t>
+  </si>
+  <si>
+    <t>PPD-</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -178,6 +188,19 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -199,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -210,6 +233,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3361,11 +3387,425 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B409EFA-EB40-3046-AB45-469039FAB82C}">
+  <dimension ref="A1:N11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="8">
+        <v>1454</v>
+      </c>
+      <c r="B1" s="8">
+        <v>72</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="9">
+        <v>12</v>
+      </c>
+      <c r="G1" s="8">
+        <v>29</v>
+      </c>
+      <c r="H1" s="8">
+        <v>2</v>
+      </c>
+      <c r="I1" s="10">
+        <v>0.375</v>
+      </c>
+      <c r="J1" s="10">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="K1" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="8">
+        <v>1455</v>
+      </c>
+      <c r="B2" s="8">
+        <v>68</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="9">
+        <v>12</v>
+      </c>
+      <c r="G2" s="8">
+        <v>28</v>
+      </c>
+      <c r="H2" s="8">
+        <v>2</v>
+      </c>
+      <c r="I2" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="J2" s="10">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="K2" s="10">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="8">
+        <v>1466</v>
+      </c>
+      <c r="B3" s="8">
+        <v>70</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="9">
+        <v>10</v>
+      </c>
+      <c r="G3" s="8">
+        <v>29</v>
+      </c>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="8">
+        <v>1525</v>
+      </c>
+      <c r="B4" s="8">
+        <v>69</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="9">
+        <v>6</v>
+      </c>
+      <c r="G4" s="8">
+        <v>28</v>
+      </c>
+      <c r="H4" s="8">
+        <v>1</v>
+      </c>
+      <c r="I4" s="10">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="J4" s="10">
+        <v>0.6875</v>
+      </c>
+      <c r="K4" s="10">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>1543</v>
+      </c>
+      <c r="B5" s="8">
+        <v>74</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="8">
+        <v>10</v>
+      </c>
+      <c r="G5" s="8">
+        <v>29</v>
+      </c>
+      <c r="H5" s="8">
+        <v>1</v>
+      </c>
+      <c r="I5" s="10">
+        <v>0.375</v>
+      </c>
+      <c r="J5" s="10">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="K5" s="10">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
+        <v>1586</v>
+      </c>
+      <c r="B6" s="8">
+        <v>71</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="8">
+        <v>14</v>
+      </c>
+      <c r="G6" s="8">
+        <v>27</v>
+      </c>
+      <c r="H6" s="8">
+        <v>2</v>
+      </c>
+      <c r="I6" s="10">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="J6" s="10">
+        <v>0.5625</v>
+      </c>
+      <c r="K6" s="10">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>1590</v>
+      </c>
+      <c r="B7" s="8">
+        <v>69</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="8">
+        <v>11</v>
+      </c>
+      <c r="G7" s="8">
+        <v>28</v>
+      </c>
+      <c r="H7" s="8">
+        <v>2</v>
+      </c>
+      <c r="I7" s="10">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="J7" s="10">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="K7" s="10">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
+        <v>1631</v>
+      </c>
+      <c r="B8" s="8">
+        <v>66</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="8">
+        <v>16</v>
+      </c>
+      <c r="G8" s="8">
+        <v>28</v>
+      </c>
+      <c r="H8" s="8">
+        <v>2</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0.375</v>
+      </c>
+      <c r="J8" s="10">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="K8" s="10">
+        <v>0.5625</v>
+      </c>
+      <c r="M8" s="10"/>
+      <c r="N8" s="8"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>1693</v>
+      </c>
+      <c r="B9" s="8">
+        <v>72</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="8">
+        <v>12</v>
+      </c>
+      <c r="G9" s="8">
+        <v>29</v>
+      </c>
+      <c r="H9" s="8">
+        <v>2</v>
+      </c>
+      <c r="I9" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="J9" s="10">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="K9" s="10">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="8">
+        <v>1720</v>
+      </c>
+      <c r="B10" s="8">
+        <v>66</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="8">
+        <v>8</v>
+      </c>
+      <c r="G10" s="8">
+        <v>29</v>
+      </c>
+      <c r="H10" s="8">
+        <v>1</v>
+      </c>
+      <c r="I10" s="10">
+        <v>0.3125</v>
+      </c>
+      <c r="J10" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="K10" s="10">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="8">
+        <v>1732</v>
+      </c>
+      <c r="B11" s="8">
+        <v>70</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="8">
+        <v>9</v>
+      </c>
+      <c r="G11" s="8">
+        <v>28</v>
+      </c>
+      <c r="H11" s="8">
+        <v>2</v>
+      </c>
+      <c r="I11" s="10">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="J11" s="10">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="K11" s="10">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD691BDA-9D3A-9C46-B4FA-85EF79BE6CF0}">
-  <dimension ref="A1:J89"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G76" sqref="G76"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5650,7 +6090,7 @@
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>1374</v>
       </c>
@@ -5682,7 +6122,7 @@
         <v>0.67708333333333337</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>1391</v>
       </c>
@@ -5714,7 +6154,7 @@
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>1102</v>
       </c>
@@ -5746,7 +6186,7 @@
         <v>0.37152777777777779</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>1215</v>
       </c>
@@ -5778,7 +6218,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>1224</v>
       </c>
@@ -5810,7 +6250,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>1260</v>
       </c>
@@ -5842,7 +6282,7 @@
         <v>0.47916666666666669</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>1326</v>
       </c>
@@ -5874,7 +6314,7 @@
         <v>0.52083333333333337</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>1348</v>
       </c>
@@ -5906,7 +6346,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>1388</v>
       </c>
@@ -5936,6 +6376,381 @@
       </c>
       <c r="J89" s="7">
         <v>0.45833333333333331</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A90" s="8">
+        <v>1454</v>
+      </c>
+      <c r="B90" s="8">
+        <v>72</v>
+      </c>
+      <c r="C90" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D90" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E90" s="9">
+        <v>12</v>
+      </c>
+      <c r="F90" s="8">
+        <v>29</v>
+      </c>
+      <c r="G90" s="8">
+        <v>2</v>
+      </c>
+      <c r="H90" s="10">
+        <v>0.375</v>
+      </c>
+      <c r="I90" s="10">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="J90" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="K90" s="10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A91" s="8">
+        <v>1455</v>
+      </c>
+      <c r="B91" s="8">
+        <v>68</v>
+      </c>
+      <c r="C91" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D91" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E91" s="9">
+        <v>12</v>
+      </c>
+      <c r="F91" s="8">
+        <v>28</v>
+      </c>
+      <c r="G91" s="8">
+        <v>2</v>
+      </c>
+      <c r="H91" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I91" s="10">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="J91" s="10">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="K91" s="10">
+        <v>0.72916666666666663</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A92" s="8">
+        <v>1466</v>
+      </c>
+      <c r="B92" s="8">
+        <v>70</v>
+      </c>
+      <c r="C92" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D92" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E92" s="9">
+        <v>10</v>
+      </c>
+      <c r="F92" s="8">
+        <v>29</v>
+      </c>
+      <c r="G92" s="8"/>
+      <c r="H92" s="8"/>
+      <c r="I92" s="8"/>
+      <c r="J92" s="8"/>
+      <c r="K92" s="8"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A93" s="8">
+        <v>1525</v>
+      </c>
+      <c r="B93" s="8">
+        <v>69</v>
+      </c>
+      <c r="C93" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D93" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E93" s="9">
+        <v>6</v>
+      </c>
+      <c r="F93" s="8">
+        <v>28</v>
+      </c>
+      <c r="G93" s="8">
+        <v>1</v>
+      </c>
+      <c r="H93" s="10">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="I93" s="10">
+        <v>0.6875</v>
+      </c>
+      <c r="J93" s="10">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="K93" s="10">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A94" s="8">
+        <v>1543</v>
+      </c>
+      <c r="B94" s="8">
+        <v>74</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E94" s="8">
+        <v>10</v>
+      </c>
+      <c r="F94" s="8">
+        <v>29</v>
+      </c>
+      <c r="G94" s="8">
+        <v>1</v>
+      </c>
+      <c r="H94" s="10">
+        <v>0.375</v>
+      </c>
+      <c r="I94" s="10">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="J94" s="10">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="K94" s="10">
+        <v>0.47916666666666669</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A95" s="8">
+        <v>1586</v>
+      </c>
+      <c r="B95" s="8">
+        <v>71</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D95" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E95" s="8">
+        <v>14</v>
+      </c>
+      <c r="F95" s="8">
+        <v>27</v>
+      </c>
+      <c r="G95" s="8">
+        <v>2</v>
+      </c>
+      <c r="H95" s="10">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="I95" s="10">
+        <v>0.5625</v>
+      </c>
+      <c r="J95" s="10">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="K95" s="10">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A96" s="8">
+        <v>1590</v>
+      </c>
+      <c r="B96" s="8">
+        <v>69</v>
+      </c>
+      <c r="C96" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E96" s="8">
+        <v>11</v>
+      </c>
+      <c r="F96" s="8">
+        <v>28</v>
+      </c>
+      <c r="G96" s="8">
+        <v>2</v>
+      </c>
+      <c r="H96" s="10">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="I96" s="10">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="J96" s="10">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="K96" s="10">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A97" s="8">
+        <v>1631</v>
+      </c>
+      <c r="B97" s="8">
+        <v>66</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D97" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E97" s="8">
+        <v>16</v>
+      </c>
+      <c r="F97" s="8">
+        <v>28</v>
+      </c>
+      <c r="G97" s="8">
+        <v>2</v>
+      </c>
+      <c r="H97" s="10">
+        <v>0.375</v>
+      </c>
+      <c r="I97" s="10">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="J97" s="10">
+        <v>0.5625</v>
+      </c>
+      <c r="K97" s="10">
+        <v>0.5625</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A98" s="8">
+        <v>1693</v>
+      </c>
+      <c r="B98" s="8">
+        <v>72</v>
+      </c>
+      <c r="C98" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D98" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E98" s="8">
+        <v>12</v>
+      </c>
+      <c r="F98" s="8">
+        <v>29</v>
+      </c>
+      <c r="G98" s="8">
+        <v>2</v>
+      </c>
+      <c r="H98" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I98" s="10">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="J98" s="10">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="K98" s="10">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A99" s="8">
+        <v>1720</v>
+      </c>
+      <c r="B99" s="8">
+        <v>66</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D99" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E99" s="8">
+        <v>8</v>
+      </c>
+      <c r="F99" s="8">
+        <v>29</v>
+      </c>
+      <c r="G99" s="8">
+        <v>1</v>
+      </c>
+      <c r="H99" s="10">
+        <v>0.3125</v>
+      </c>
+      <c r="I99" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="J99" s="10">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="K99" s="10">
+        <v>0.35416666666666669</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A100" s="8">
+        <v>1732</v>
+      </c>
+      <c r="B100" s="8">
+        <v>70</v>
+      </c>
+      <c r="C100" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E100" s="8">
+        <v>9</v>
+      </c>
+      <c r="F100" s="8">
+        <v>28</v>
+      </c>
+      <c r="G100" s="8">
+        <v>2</v>
+      </c>
+      <c r="H100" s="10">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="I100" s="10">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="J100" s="10">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="K100" s="10">
+        <v>0.54166666666666663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
creating figures for publication
</commit_message>
<xml_diff>
--- a/data/data_gridsearch_subjects.xlsx
+++ b/data/data_gridsearch_subjects.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hmupm-my.sharepoint.com/personal/bjoern_meder_hmu-potsdam_de/Documents/_Projekte/gridsearch Parkinson/2024 gridSearch Parkinson/06_github_repo/gridsearch_parkinsons/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{30E631F0-5369-664A-9279-3B69550168D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5D55E68-0D97-524A-9E8C-7ADA535822E6}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{30E631F0-5369-664A-9279-3B69550168D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6667688-CF58-094A-ABDD-1705C2D2DDCC}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{9551D2BD-E314-0446-B93E-CE842B5EA9E5}"/>
   </bookViews>
@@ -251,6 +251,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3802,10 +3806,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD691BDA-9D3A-9C46-B4FA-85EF79BE6CF0}">
-  <dimension ref="A1:K100"/>
+  <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="K68" sqref="K1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6090,7 +6094,7 @@
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>1374</v>
       </c>
@@ -6122,7 +6126,7 @@
         <v>0.67708333333333337</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>1391</v>
       </c>
@@ -6154,7 +6158,7 @@
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>1102</v>
       </c>
@@ -6186,7 +6190,7 @@
         <v>0.37152777777777779</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>1215</v>
       </c>
@@ -6218,7 +6222,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>1224</v>
       </c>
@@ -6250,7 +6254,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>1260</v>
       </c>
@@ -6282,7 +6286,7 @@
         <v>0.47916666666666669</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>1326</v>
       </c>
@@ -6314,7 +6318,7 @@
         <v>0.52083333333333337</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>1348</v>
       </c>
@@ -6346,7 +6350,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>1388</v>
       </c>
@@ -6378,7 +6382,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="8">
         <v>1454</v>
       </c>
@@ -6409,11 +6413,8 @@
       <c r="J90" s="10">
         <v>0.5</v>
       </c>
-      <c r="K90" s="10">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="8">
         <v>1455</v>
       </c>
@@ -6444,11 +6445,8 @@
       <c r="J91" s="10">
         <v>0.72916666666666663</v>
       </c>
-      <c r="K91" s="10">
-        <v>0.72916666666666663</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="8">
         <v>1466</v>
       </c>
@@ -6471,9 +6469,8 @@
       <c r="H92" s="8"/>
       <c r="I92" s="8"/>
       <c r="J92" s="8"/>
-      <c r="K92" s="8"/>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="8">
         <v>1525</v>
       </c>
@@ -6504,11 +6501,8 @@
       <c r="J93" s="10">
         <v>0.70833333333333337</v>
       </c>
-      <c r="K93" s="10">
-        <v>0.70833333333333337</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="8">
         <v>1543</v>
       </c>
@@ -6539,11 +6533,8 @@
       <c r="J94" s="10">
         <v>0.47916666666666669</v>
       </c>
-      <c r="K94" s="10">
-        <v>0.47916666666666669</v>
-      </c>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="8">
         <v>1586</v>
       </c>
@@ -6574,11 +6565,8 @@
       <c r="J95" s="10">
         <v>0.58333333333333337</v>
       </c>
-      <c r="K95" s="10">
-        <v>0.58333333333333337</v>
-      </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="8">
         <v>1590</v>
       </c>
@@ -6609,11 +6597,8 @@
       <c r="J96" s="10">
         <v>0.41666666666666669</v>
       </c>
-      <c r="K96" s="10">
-        <v>0.41666666666666669</v>
-      </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="8">
         <v>1631</v>
       </c>
@@ -6644,11 +6629,8 @@
       <c r="J97" s="10">
         <v>0.5625</v>
       </c>
-      <c r="K97" s="10">
-        <v>0.5625</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="8">
         <v>1693</v>
       </c>
@@ -6679,11 +6661,8 @@
       <c r="J98" s="10">
         <v>0.70833333333333337</v>
       </c>
-      <c r="K98" s="10">
-        <v>0.70833333333333337</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="8">
         <v>1720</v>
       </c>
@@ -6714,11 +6693,8 @@
       <c r="J99" s="10">
         <v>0.35416666666666669</v>
       </c>
-      <c r="K99" s="10">
-        <v>0.35416666666666669</v>
-      </c>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="8">
         <v>1732</v>
       </c>
@@ -6747,9 +6723,6 @@
         <v>0.52083333333333337</v>
       </c>
       <c r="J100" s="10">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="K100" s="10">
         <v>0.54166666666666663</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added last 3 data points and re-run behavioral analyses
</commit_message>
<xml_diff>
--- a/data/data_gridsearch_subjects.xlsx
+++ b/data/data_gridsearch_subjects.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hmupm-my.sharepoint.com/personal/bjoern_meder_hmu-potsdam_de/Documents/_Projekte/gridsearch Parkinson/2024 gridSearch Parkinson/06_github_repo/gridsearch_parkinsons/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{30E631F0-5369-664A-9279-3B69550168D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6667688-CF58-094A-ABDD-1705C2D2DDCC}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="8_{30E631F0-5369-664A-9279-3B69550168D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4E81D2E-1046-5842-8FDC-D611DC7296C2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="3" xr2:uid="{9551D2BD-E314-0446-B93E-CE842B5EA9E5}"/>
+    <workbookView xWindow="52480" yWindow="1080" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{9551D2BD-E314-0446-B93E-CE842B5EA9E5}"/>
   </bookViews>
   <sheets>
     <sheet name="batch1" sheetId="2" r:id="rId1"/>
     <sheet name="batch2" sheetId="1" r:id="rId2"/>
     <sheet name="batch3" sheetId="4" r:id="rId3"/>
-    <sheet name="all" sheetId="3" r:id="rId4"/>
+    <sheet name="batch4" sheetId="5" r:id="rId4"/>
+    <sheet name="all" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="gridsearch_subject_data" localSheetId="3">all!$A$1:$J$63</definedName>
+    <definedName name="gridsearch_subject_data" localSheetId="4">all!$A$1:$J$63</definedName>
     <definedName name="gridsearch_subject_data" localSheetId="0">batch1!$A$1:$J$63</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -80,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="20">
   <si>
     <t>id</t>
   </si>
@@ -586,7 +587,7 @@
   <sheetViews>
     <sheetView zoomScale="135" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C62" sqref="A1:J63"/>
+      <selection pane="bottomLeft" sqref="A1:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3395,7 +3396,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K11"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3805,11 +3806,258 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F1F1455-D09F-AF48-AB82-E18289743AA1}">
+  <dimension ref="A1:K19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1532</v>
+      </c>
+      <c r="B1">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="6">
+        <v>12</v>
+      </c>
+      <c r="F1">
+        <v>27</v>
+      </c>
+      <c r="J1" s="7">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1596</v>
+      </c>
+      <c r="B2">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>16</v>
+      </c>
+      <c r="F2">
+        <v>28</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="I2" s="7">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="J2" s="7">
+        <v>0.54861111111111116</v>
+      </c>
+      <c r="K2" s="7"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1663</v>
+      </c>
+      <c r="B3">
+        <v>70</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>11</v>
+      </c>
+      <c r="F3">
+        <v>29</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD691BDA-9D3A-9C46-B4FA-85EF79BE6CF0}">
-  <dimension ref="A1:J100"/>
+  <dimension ref="A1:J103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="K68" sqref="K1:M1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="K76" sqref="K1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5678,7 +5926,7 @@
         <v>66</v>
       </c>
       <c r="C64" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D64" t="s">
         <v>11</v>
@@ -5701,7 +5949,7 @@
         <v>74</v>
       </c>
       <c r="C65" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D65" t="s">
         <v>11</v>
@@ -5770,7 +6018,7 @@
         <v>67</v>
       </c>
       <c r="C68" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D68" t="s">
         <v>11</v>
@@ -5816,7 +6064,7 @@
         <v>68</v>
       </c>
       <c r="C70" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D70" t="s">
         <v>11</v>
@@ -5839,7 +6087,7 @@
         <v>66</v>
       </c>
       <c r="C71" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D71" t="s">
         <v>11</v>
@@ -5859,7 +6107,7 @@
         <v>70</v>
       </c>
       <c r="C72" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D72" t="s">
         <v>11</v>
@@ -5928,7 +6176,7 @@
         <v>63</v>
       </c>
       <c r="C75" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D75" t="s">
         <v>11</v>
@@ -6006,7 +6254,7 @@
         <v>61</v>
       </c>
       <c r="C78" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D78" t="s">
         <v>13</v>
@@ -6102,7 +6350,7 @@
         <v>64</v>
       </c>
       <c r="C81" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D81" t="s">
         <v>13</v>
@@ -6166,7 +6414,7 @@
         <v>72</v>
       </c>
       <c r="C83" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D83" t="s">
         <v>15</v>
@@ -6198,7 +6446,7 @@
         <v>71</v>
       </c>
       <c r="C84" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D84" t="s">
         <v>15</v>
@@ -6326,7 +6574,7 @@
         <v>72</v>
       </c>
       <c r="C88" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D88" t="s">
         <v>15</v>
@@ -6358,7 +6606,7 @@
         <v>64</v>
       </c>
       <c r="C89" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D89" t="s">
         <v>15</v>
@@ -6390,7 +6638,7 @@
         <v>72</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D90" s="8" t="s">
         <v>15</v>
@@ -6454,7 +6702,7 @@
         <v>70</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D92" s="8" t="s">
         <v>11</v>
@@ -6478,7 +6726,7 @@
         <v>69</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D93" s="8" t="s">
         <v>13</v>
@@ -6510,7 +6758,7 @@
         <v>74</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D94" s="8" t="s">
         <v>15</v>
@@ -6638,7 +6886,7 @@
         <v>72</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D98" s="8" t="s">
         <v>13</v>
@@ -6724,6 +6972,93 @@
       </c>
       <c r="J100" s="10">
         <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>1532</v>
+      </c>
+      <c r="B101">
+        <v>72</v>
+      </c>
+      <c r="C101" t="s">
+        <v>14</v>
+      </c>
+      <c r="D101" t="s">
+        <v>11</v>
+      </c>
+      <c r="E101" s="6">
+        <v>12</v>
+      </c>
+      <c r="F101">
+        <v>27</v>
+      </c>
+      <c r="J101" s="7">
+        <v>0.58333333333333337</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>1596</v>
+      </c>
+      <c r="B102">
+        <v>68</v>
+      </c>
+      <c r="C102" t="s">
+        <v>10</v>
+      </c>
+      <c r="D102" t="s">
+        <v>13</v>
+      </c>
+      <c r="E102">
+        <v>16</v>
+      </c>
+      <c r="F102">
+        <v>28</v>
+      </c>
+      <c r="G102">
+        <v>2</v>
+      </c>
+      <c r="H102" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="I102" s="7">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="J102" s="7">
+        <v>0.54861111111111116</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>1663</v>
+      </c>
+      <c r="B103">
+        <v>70</v>
+      </c>
+      <c r="C103" t="s">
+        <v>10</v>
+      </c>
+      <c r="D103" t="s">
+        <v>13</v>
+      </c>
+      <c r="E103">
+        <v>11</v>
+      </c>
+      <c r="F103">
+        <v>29</v>
+      </c>
+      <c r="G103">
+        <v>1</v>
+      </c>
+      <c r="H103" s="7">
+        <v>0.375</v>
+      </c>
+      <c r="I103" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="J103" s="7">
+        <v>0.49305555555555558</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated with last 2 subjects
</commit_message>
<xml_diff>
--- a/data/data_gridsearch_subjects.xlsx
+++ b/data/data_gridsearch_subjects.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hmupm-my.sharepoint.com/personal/bjoern_meder_hmu-potsdam_de/Documents/_Projekte/gridsearch Parkinson/2024 gridSearch Parkinson/06_github_repo/gridsearch_parkinsons/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{30E631F0-5369-664A-9279-3B69550168D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4E81D2E-1046-5842-8FDC-D611DC7296C2}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="8_{30E631F0-5369-664A-9279-3B69550168D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF7D6E56-C05D-9046-8486-C17DA8EE2F27}"/>
   <bookViews>
     <workbookView xWindow="52480" yWindow="1080" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{9551D2BD-E314-0446-B93E-CE842B5EA9E5}"/>
   </bookViews>
@@ -23,7 +23,7 @@
     <definedName name="gridsearch_subject_data" localSheetId="4">all!$A$1:$J$63</definedName>
     <definedName name="gridsearch_subject_data" localSheetId="0">batch1!$A$1:$J$63</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="20">
   <si>
     <t>id</t>
   </si>
@@ -3396,7 +3396,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3409,7 +3409,7 @@
         <v>72</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>17</v>
@@ -3483,7 +3483,7 @@
         <v>70</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>11</v>
@@ -3512,7 +3512,7 @@
         <v>69</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>17</v>
@@ -3549,7 +3549,7 @@
         <v>74</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>18</v>
@@ -3697,7 +3697,7 @@
         <v>72</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>17</v>
@@ -3810,7 +3810,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3846,7 +3846,7 @@
         <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
@@ -3879,7 +3879,7 @@
         <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -3903,6 +3903,76 @@
         <v>0.49305555555555558</v>
       </c>
       <c r="K3" s="7"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1706</v>
+      </c>
+      <c r="B4">
+        <v>72</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>28</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="J4" s="7">
+        <v>0.40625</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1722</v>
+      </c>
+      <c r="B5">
+        <v>74</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>29</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0.67708333333333337</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
@@ -4054,10 +4124,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD691BDA-9D3A-9C46-B4FA-85EF79BE6CF0}">
-  <dimension ref="A1:J103"/>
+  <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="K76" sqref="K1:P1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="R99" sqref="R99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7061,6 +7131,70 @@
         <v>0.49305555555555558</v>
       </c>
     </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>1706</v>
+      </c>
+      <c r="B104">
+        <v>72</v>
+      </c>
+      <c r="C104" t="s">
+        <v>10</v>
+      </c>
+      <c r="D104" t="s">
+        <v>15</v>
+      </c>
+      <c r="E104">
+        <v>10</v>
+      </c>
+      <c r="F104">
+        <v>28</v>
+      </c>
+      <c r="G104">
+        <v>2</v>
+      </c>
+      <c r="H104" s="7">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I104" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="J104" s="7">
+        <v>0.40625</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>1722</v>
+      </c>
+      <c r="B105">
+        <v>74</v>
+      </c>
+      <c r="C105" t="s">
+        <v>10</v>
+      </c>
+      <c r="D105" t="s">
+        <v>13</v>
+      </c>
+      <c r="E105">
+        <v>7</v>
+      </c>
+      <c r="F105">
+        <v>29</v>
+      </c>
+      <c r="G105">
+        <v>1</v>
+      </c>
+      <c r="H105" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I105" s="7">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J105" s="7">
+        <v>0.67708333333333337</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
included LEDD data in Quarto and HTML file
</commit_message>
<xml_diff>
--- a/data/data_gridsearch_subjects.xlsx
+++ b/data/data_gridsearch_subjects.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29429"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hmupm-my.sharepoint.com/personal/bjoern_meder_hmu-potsdam_de/Documents/_Projekte/gridsearch Parkinson/2024 gridSearch Parkinson/06_github_repo/gridsearch_parkinsons/data/"/>
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="73" documentId="8_{30E631F0-5369-664A-9279-3B69550168D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF7D6E56-C05D-9046-8486-C17DA8EE2F27}"/>
   <bookViews>
-    <workbookView xWindow="52480" yWindow="1080" windowWidth="30240" windowHeight="18880" activeTab="4" xr2:uid="{9551D2BD-E314-0446-B93E-CE842B5EA9E5}"/>
+    <workbookView xWindow="52480" yWindow="1080" windowWidth="30240" windowHeight="18880" firstSheet="4" activeTab="4" xr2:uid="{9551D2BD-E314-0446-B93E-CE842B5EA9E5}"/>
   </bookViews>
   <sheets>
     <sheet name="batch1" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <definedName name="gridsearch_subject_data" localSheetId="4">all!$A$1:$J$63</definedName>
     <definedName name="gridsearch_subject_data" localSheetId="0">batch1!$A$1:$J$63</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191028" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -116,12 +116,6 @@
     <t>f</t>
   </si>
   <si>
-    <t>PNP</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>PD-</t>
   </si>
   <si>
@@ -129,6 +123,12 @@
   </si>
   <si>
     <t>PD+</t>
+  </si>
+  <si>
+    <t>PNP</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
   <si>
     <t>w</t>
@@ -147,7 +147,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -239,7 +239,7 @@
     <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -252,10 +252,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -590,21 +586,21 @@
       <selection pane="bottomLeft" sqref="A1:J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.625" customWidth="1"/>
+    <col min="3" max="3" width="8.875" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="5.83203125" customWidth="1"/>
-    <col min="6" max="6" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.875" customWidth="1"/>
+    <col min="6" max="6" width="6.375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.375" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
     <col min="10" max="10" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -636,7 +632,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" s="3">
         <v>168</v>
       </c>
@@ -647,7 +643,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E2" s="3">
         <v>2</v>
@@ -668,7 +664,7 @@
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="3">
         <v>212</v>
       </c>
@@ -676,10 +672,10 @@
         <v>78</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -700,7 +696,7 @@
         <v>0.53472222222222221</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" s="3">
         <v>227</v>
       </c>
@@ -711,7 +707,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E4" s="3">
         <v>12</v>
@@ -732,7 +728,7 @@
         <v>0.48958333333333331</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" s="3">
         <v>239</v>
       </c>
@@ -743,7 +739,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E5" s="3">
         <v>4</v>
@@ -764,7 +760,7 @@
         <v>0.55208333333333337</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" s="3">
         <v>271</v>
       </c>
@@ -772,10 +768,10 @@
         <v>64</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E6" s="3">
         <v>11</v>
@@ -796,7 +792,7 @@
         <v>0.47916666666666669</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" s="3">
         <v>275</v>
       </c>
@@ -804,10 +800,10 @@
         <v>67</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E7" s="3">
         <v>6</v>
@@ -828,7 +824,7 @@
         <v>0.53472222222222221</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" s="3">
         <v>279</v>
       </c>
@@ -839,7 +835,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E8" s="3">
         <v>13</v>
@@ -860,7 +856,7 @@
         <v>0.55555555555555558</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" s="3">
         <v>333</v>
       </c>
@@ -868,10 +864,10 @@
         <v>79</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E9" s="3">
         <v>9</v>
@@ -892,7 +888,7 @@
         <v>0.52083333333333337</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="A10" s="3">
         <v>418</v>
       </c>
@@ -903,7 +899,7 @@
         <v>10</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E10" s="3">
         <v>9</v>
@@ -924,7 +920,7 @@
         <v>0.52083333333333337</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" s="3">
         <v>481</v>
       </c>
@@ -935,7 +931,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E11" s="3">
         <v>4</v>
@@ -956,7 +952,7 @@
         <v>0.52083333333333337</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" s="3">
         <v>556</v>
       </c>
@@ -964,10 +960,10 @@
         <v>69</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E12" s="3">
         <v>12</v>
@@ -988,7 +984,7 @@
         <v>0.51041666666666663</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13" s="3">
         <v>607</v>
       </c>
@@ -996,10 +992,10 @@
         <v>77</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E13" s="3">
         <v>9</v>
@@ -1020,7 +1016,7 @@
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" s="3">
         <v>656</v>
       </c>
@@ -1031,7 +1027,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E14" s="3">
         <v>3</v>
@@ -1052,7 +1048,7 @@
         <v>0.50694444444444442</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" s="3">
         <v>661</v>
       </c>
@@ -1060,10 +1056,10 @@
         <v>59</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E15" s="3">
         <v>11</v>
@@ -1084,7 +1080,7 @@
         <v>0.40972222222222221</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" s="3">
         <v>738</v>
       </c>
@@ -1092,10 +1088,10 @@
         <v>69</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E16" s="3">
         <v>1</v>
@@ -1116,7 +1112,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10">
       <c r="A17" s="3">
         <v>775</v>
       </c>
@@ -1124,10 +1120,10 @@
         <v>74</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E17" s="3">
         <v>7</v>
@@ -1148,7 +1144,7 @@
         <v>0.56944444444444442</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10">
       <c r="A18" s="3">
         <v>816</v>
       </c>
@@ -1156,10 +1152,10 @@
         <v>68</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E18" s="3">
         <v>4</v>
@@ -1180,7 +1176,7 @@
         <v>0.52083333333333337</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10">
       <c r="A19" s="3">
         <v>923</v>
       </c>
@@ -1188,10 +1184,10 @@
         <v>63</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E19" s="3">
         <v>7</v>
@@ -1212,7 +1208,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10">
       <c r="A20" s="3">
         <v>963</v>
       </c>
@@ -1223,7 +1219,7 @@
         <v>10</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E20" s="3">
         <v>8</v>
@@ -1244,7 +1240,7 @@
         <v>0.47916666666666669</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10">
       <c r="A21" s="3">
         <v>983</v>
       </c>
@@ -1255,7 +1251,7 @@
         <v>10</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E21" s="3">
         <v>10</v>
@@ -1276,7 +1272,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10">
       <c r="A22" s="3">
         <v>274</v>
       </c>
@@ -1284,10 +1280,10 @@
         <v>56</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E22" s="3">
         <v>7</v>
@@ -1308,7 +1304,7 @@
         <v>0.59722222222222221</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10">
       <c r="A23" s="3">
         <v>285</v>
       </c>
@@ -1319,7 +1315,7 @@
         <v>10</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E23" s="3">
         <v>4</v>
@@ -1340,7 +1336,7 @@
         <v>0.4236111111111111</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10">
       <c r="A24" s="3">
         <v>317</v>
       </c>
@@ -1351,7 +1347,7 @@
         <v>10</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E24" s="3">
         <v>7</v>
@@ -1372,7 +1368,7 @@
         <v>0.61458333333333337</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10">
       <c r="A25" s="3">
         <v>334</v>
       </c>
@@ -1383,7 +1379,7 @@
         <v>10</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E25" s="3">
         <v>6</v>
@@ -1404,7 +1400,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10">
       <c r="A26" s="3">
         <v>380</v>
       </c>
@@ -1412,10 +1408,10 @@
         <v>73</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E26" s="3">
         <v>8</v>
@@ -1436,7 +1432,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10">
       <c r="A27" s="3">
         <v>393</v>
       </c>
@@ -1444,10 +1440,10 @@
         <v>69</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E27" s="3">
         <v>17</v>
@@ -1468,7 +1464,7 @@
         <v>0.47916666666666669</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10">
       <c r="A28" s="3">
         <v>406</v>
       </c>
@@ -1476,10 +1472,10 @@
         <v>62</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E28" s="3">
         <v>11</v>
@@ -1500,7 +1496,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10">
       <c r="A29" s="3">
         <v>445</v>
       </c>
@@ -1511,7 +1507,7 @@
         <v>10</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E29" s="3">
         <v>14</v>
@@ -1532,7 +1528,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10">
       <c r="A30" s="3">
         <v>535</v>
       </c>
@@ -1543,7 +1539,7 @@
         <v>10</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E30" s="3">
         <v>11</v>
@@ -1564,7 +1560,7 @@
         <v>0.47916666666666669</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10">
       <c r="A31" s="3">
         <v>595</v>
       </c>
@@ -1575,7 +1571,7 @@
         <v>10</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E31" s="3">
         <v>8</v>
@@ -1596,7 +1592,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10">
       <c r="A32" s="3">
         <v>633</v>
       </c>
@@ -1604,10 +1600,10 @@
         <v>61</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E32" s="3">
         <v>12</v>
@@ -1628,7 +1624,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10">
       <c r="A33" s="3">
         <v>659</v>
       </c>
@@ -1639,7 +1635,7 @@
         <v>10</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E33" s="3">
         <v>14</v>
@@ -1660,7 +1656,7 @@
         <v>0.46875</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10">
       <c r="A34" s="3">
         <v>717</v>
       </c>
@@ -1671,7 +1667,7 @@
         <v>10</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E34" s="3">
         <v>11</v>
@@ -1692,7 +1688,7 @@
         <v>0.44791666666666669</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10">
       <c r="A35" s="3">
         <v>730</v>
       </c>
@@ -1700,10 +1696,10 @@
         <v>70</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E35" s="3">
         <v>3</v>
@@ -1724,7 +1720,7 @@
         <v>0.40625</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10">
       <c r="A36" s="3">
         <v>739</v>
       </c>
@@ -1735,7 +1731,7 @@
         <v>10</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E36" s="3">
         <v>3</v>
@@ -1756,7 +1752,7 @@
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10">
       <c r="A37" s="3">
         <v>753</v>
       </c>
@@ -1764,10 +1760,10 @@
         <v>67</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E37" s="3">
         <v>6</v>
@@ -1788,7 +1784,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10">
       <c r="A38" s="3">
         <v>787</v>
       </c>
@@ -1796,10 +1792,10 @@
         <v>61</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E38" s="3">
         <v>6</v>
@@ -1820,7 +1816,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10">
       <c r="A39" s="3">
         <v>839</v>
       </c>
@@ -1828,10 +1824,10 @@
         <v>55</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E39" s="3">
         <v>3</v>
@@ -1852,7 +1848,7 @@
         <v>0.51041666666666663</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10">
       <c r="A40" s="3">
         <v>862</v>
       </c>
@@ -1860,10 +1856,10 @@
         <v>57</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E40" s="3">
         <v>3</v>
@@ -1884,7 +1880,7 @@
         <v>0.47916666666666669</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10">
       <c r="A41" s="3">
         <v>888</v>
       </c>
@@ -1895,7 +1891,7 @@
         <v>10</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E41" s="3">
         <v>12</v>
@@ -1916,7 +1912,7 @@
         <v>0.40277777777777779</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10">
       <c r="A42" s="3">
         <v>897</v>
       </c>
@@ -1924,10 +1920,10 @@
         <v>53</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E42" s="3">
         <v>4</v>
@@ -1948,7 +1944,7 @@
         <v>0.60416666666666663</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10">
       <c r="A43" s="3">
         <v>976</v>
       </c>
@@ -1959,7 +1955,7 @@
         <v>10</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E43" s="3">
         <v>5</v>
@@ -1980,7 +1976,7 @@
         <v>0.59722222222222221</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10">
       <c r="A44" s="3">
         <v>111</v>
       </c>
@@ -1991,7 +1987,7 @@
         <v>10</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E44" s="3">
         <v>12</v>
@@ -2000,19 +1996,19 @@
         <v>30</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" s="3">
         <v>115</v>
       </c>
@@ -2023,7 +2019,7 @@
         <v>10</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E45" s="3">
         <v>11</v>
@@ -2032,19 +2028,19 @@
         <v>27</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" s="3">
         <v>117</v>
       </c>
@@ -2055,7 +2051,7 @@
         <v>10</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E46" s="3">
         <v>8</v>
@@ -2064,19 +2060,19 @@
         <v>30</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" s="3">
         <v>234</v>
       </c>
@@ -2087,7 +2083,7 @@
         <v>10</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E47" s="3">
         <v>12</v>
@@ -2096,19 +2092,19 @@
         <v>29</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48" s="3">
         <v>250</v>
       </c>
@@ -2116,10 +2112,10 @@
         <v>72</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E48" s="3">
         <v>11</v>
@@ -2128,19 +2124,19 @@
         <v>28</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" s="3">
         <v>256</v>
       </c>
@@ -2151,7 +2147,7 @@
         <v>10</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E49" s="3">
         <v>5</v>
@@ -2160,19 +2156,19 @@
         <v>30</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50" s="3">
         <v>353</v>
       </c>
@@ -2180,10 +2176,10 @@
         <v>61</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E50" s="3">
         <v>4</v>
@@ -2192,19 +2188,19 @@
         <v>29</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51" s="3">
         <v>367</v>
       </c>
@@ -2215,7 +2211,7 @@
         <v>10</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E51" s="3">
         <v>3</v>
@@ -2224,19 +2220,19 @@
         <v>30</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52" s="3">
         <v>422</v>
       </c>
@@ -2244,10 +2240,10 @@
         <v>61</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E52" s="3">
         <v>11</v>
@@ -2256,19 +2252,19 @@
         <v>30</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53" s="3">
         <v>427</v>
       </c>
@@ -2276,10 +2272,10 @@
         <v>61</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E53" s="3">
         <v>1</v>
@@ -2288,19 +2284,19 @@
         <v>27</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I53" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J53" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54" s="3">
         <v>476</v>
       </c>
@@ -2308,10 +2304,10 @@
         <v>77</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E54" s="3">
         <v>10</v>
@@ -2320,19 +2316,19 @@
         <v>29</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I54" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J54" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55" s="3">
         <v>488</v>
       </c>
@@ -2343,7 +2339,7 @@
         <v>10</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E55" s="3">
         <v>14</v>
@@ -2352,19 +2348,19 @@
         <v>29</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J55" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56" s="3">
         <v>495</v>
       </c>
@@ -2375,7 +2371,7 @@
         <v>10</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E56" s="3">
         <v>7</v>
@@ -2384,19 +2380,19 @@
         <v>29</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57" s="3">
         <v>512</v>
       </c>
@@ -2407,7 +2403,7 @@
         <v>10</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E57" s="3">
         <v>9</v>
@@ -2416,19 +2412,19 @@
         <v>30</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58" s="3">
         <v>541</v>
       </c>
@@ -2439,7 +2435,7 @@
         <v>10</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E58" s="3">
         <v>13</v>
@@ -2448,19 +2444,19 @@
         <v>29</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59" s="3">
         <v>553</v>
       </c>
@@ -2471,7 +2467,7 @@
         <v>10</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E59" s="3">
         <v>5</v>
@@ -2480,19 +2476,19 @@
         <v>29</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60" s="3">
         <v>589</v>
       </c>
@@ -2500,10 +2496,10 @@
         <v>72</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E60" s="3">
         <v>3</v>
@@ -2512,19 +2508,19 @@
         <v>30</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61" s="3">
         <v>773</v>
       </c>
@@ -2535,7 +2531,7 @@
         <v>10</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E61" s="3">
         <v>10</v>
@@ -2544,19 +2540,19 @@
         <v>30</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62" s="3">
         <v>859</v>
       </c>
@@ -2567,7 +2563,7 @@
         <v>10</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E62" s="3">
         <v>8</v>
@@ -2576,19 +2572,19 @@
         <v>28</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63" s="3">
         <v>915</v>
       </c>
@@ -2596,10 +2592,10 @@
         <v>54</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E63" s="3">
         <v>5</v>
@@ -2608,16 +2604,16 @@
         <v>29</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -2637,9 +2633,9 @@
       <selection sqref="A1:J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2671,7 +2667,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1154</v>
       </c>
@@ -2682,7 +2678,7 @@
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E2" s="6">
         <v>7</v>
@@ -2694,7 +2690,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>1155</v>
       </c>
@@ -2705,7 +2701,7 @@
         <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E3" s="6">
         <v>10</v>
@@ -2717,7 +2713,7 @@
         <v>0.3888888888888889</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>1175</v>
       </c>
@@ -2725,10 +2721,10 @@
         <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E4" s="6">
         <v>5</v>
@@ -2740,7 +2736,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>1194</v>
       </c>
@@ -2748,10 +2744,10 @@
         <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E5" s="6">
         <v>6</v>
@@ -2763,7 +2759,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>1196</v>
       </c>
@@ -2774,7 +2770,7 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E6" s="6">
         <v>12</v>
@@ -2786,7 +2782,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>1214</v>
       </c>
@@ -2794,10 +2790,10 @@
         <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E7" s="6">
         <v>11</v>
@@ -2809,7 +2805,7 @@
         <v>0.52083333333333337</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>1288</v>
       </c>
@@ -2820,7 +2816,7 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E8" s="6">
         <v>5</v>
@@ -2832,7 +2828,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>1300</v>
       </c>
@@ -2843,7 +2839,7 @@
         <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E9" s="6">
         <v>9</v>
@@ -2852,7 +2848,7 @@
         <v>0.47916666666666669</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>1319</v>
       </c>
@@ -2863,7 +2859,7 @@
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E10" s="6">
         <v>9</v>
@@ -2875,7 +2871,7 @@
         <v>0.6875</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>1325</v>
       </c>
@@ -2883,10 +2879,10 @@
         <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E11" s="6">
         <v>11</v>
@@ -2898,7 +2894,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>1345</v>
       </c>
@@ -2906,10 +2902,10 @@
         <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E12" s="6">
         <v>13</v>
@@ -2921,7 +2917,7 @@
         <v>0.52083333333333337</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>1379</v>
       </c>
@@ -2932,7 +2928,7 @@
         <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E13" s="6">
         <v>5</v>
@@ -2944,7 +2940,7 @@
         <v>0.40625</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>1452</v>
       </c>
@@ -2952,10 +2948,10 @@
         <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E14" s="6">
         <v>10</v>
@@ -2970,7 +2966,7 @@
         <v>0.60416666666666663</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>1164</v>
       </c>
@@ -2978,10 +2974,10 @@
         <v>67</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E15" s="6">
         <v>11</v>
@@ -3002,7 +2998,7 @@
         <v>0.49305555555555558</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>1176</v>
       </c>
@@ -3013,7 +3009,7 @@
         <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E16" s="6">
         <v>13</v>
@@ -3034,7 +3030,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>1266</v>
       </c>
@@ -3042,10 +3038,10 @@
         <v>70</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E17" s="6">
         <v>10</v>
@@ -3066,7 +3062,7 @@
         <v>0.49305555555555558</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>1312</v>
       </c>
@@ -3074,10 +3070,10 @@
         <v>71</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E18" s="6">
         <v>8</v>
@@ -3098,7 +3094,7 @@
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>1374</v>
       </c>
@@ -3109,7 +3105,7 @@
         <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E19" s="6">
         <v>7</v>
@@ -3130,7 +3126,7 @@
         <v>0.67708333333333337</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>1391</v>
       </c>
@@ -3138,10 +3134,10 @@
         <v>69</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E20" s="6">
         <v>4</v>
@@ -3162,7 +3158,7 @@
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>1102</v>
       </c>
@@ -3173,7 +3169,7 @@
         <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E21" s="6">
         <v>11</v>
@@ -3194,7 +3190,7 @@
         <v>0.37152777777777779</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>1215</v>
       </c>
@@ -3205,7 +3201,7 @@
         <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E22" s="6">
         <v>10</v>
@@ -3226,7 +3222,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>1224</v>
       </c>
@@ -3234,10 +3230,10 @@
         <v>69</v>
       </c>
       <c r="C23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E23" s="6">
         <v>9</v>
@@ -3258,7 +3254,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>1260</v>
       </c>
@@ -3266,10 +3262,10 @@
         <v>65</v>
       </c>
       <c r="C24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E24" s="6">
         <v>9</v>
@@ -3290,7 +3286,7 @@
         <v>0.47916666666666669</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>1326</v>
       </c>
@@ -3298,10 +3294,10 @@
         <v>66</v>
       </c>
       <c r="C25" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E25" s="6">
         <v>6</v>
@@ -3322,7 +3318,7 @@
         <v>0.52083333333333337</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>1348</v>
       </c>
@@ -3333,7 +3329,7 @@
         <v>16</v>
       </c>
       <c r="D26" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E26" s="6">
         <v>11</v>
@@ -3354,7 +3350,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>1388</v>
       </c>
@@ -3365,7 +3361,7 @@
         <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E27" s="6">
         <v>9</v>
@@ -3399,9 +3395,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="8">
         <v>1454</v>
       </c>
@@ -3438,7 +3434,7 @@
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" s="8">
         <v>1455</v>
       </c>
@@ -3446,7 +3442,7 @@
         <v>68</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>17</v>
@@ -3475,7 +3471,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3" s="8">
         <v>1466</v>
       </c>
@@ -3486,10 +3482,10 @@
         <v>10</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F3" s="9">
         <v>10</v>
@@ -3504,7 +3500,7 @@
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="A4" s="8">
         <v>1525</v>
       </c>
@@ -3541,7 +3537,7 @@
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="A5" s="8">
         <v>1543</v>
       </c>
@@ -3578,7 +3574,7 @@
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" s="8">
         <v>1586</v>
       </c>
@@ -3586,7 +3582,7 @@
         <v>71</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>17</v>
@@ -3615,7 +3611,7 @@
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7" s="8">
         <v>1590</v>
       </c>
@@ -3623,7 +3619,7 @@
         <v>69</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>17</v>
@@ -3652,7 +3648,7 @@
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="A8" s="8">
         <v>1631</v>
       </c>
@@ -3660,7 +3656,7 @@
         <v>66</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>17</v>
@@ -3689,7 +3685,7 @@
       <c r="M8" s="10"/>
       <c r="N8" s="8"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="A9" s="8">
         <v>1693</v>
       </c>
@@ -3726,7 +3722,7 @@
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14">
       <c r="A10" s="8">
         <v>1720</v>
       </c>
@@ -3734,7 +3730,7 @@
         <v>66</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>17</v>
@@ -3763,7 +3759,7 @@
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14">
       <c r="A11" s="8">
         <v>1732</v>
       </c>
@@ -3771,7 +3767,7 @@
         <v>70</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>17</v>
@@ -3813,9 +3809,9 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1">
         <v>1532</v>
       </c>
@@ -3823,10 +3819,10 @@
         <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E1" s="6">
         <v>12</v>
@@ -3838,7 +3834,7 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1596</v>
       </c>
@@ -3849,7 +3845,7 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E2">
         <v>16</v>
@@ -3871,7 +3867,7 @@
       </c>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>1663</v>
       </c>
@@ -3882,7 +3878,7 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E3">
         <v>11</v>
@@ -3904,7 +3900,7 @@
       </c>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>1706</v>
       </c>
@@ -3915,7 +3911,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4">
         <v>10</v>
@@ -3936,7 +3932,7 @@
         <v>0.40625</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>1722</v>
       </c>
@@ -3947,7 +3943,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E5">
         <v>7</v>
@@ -3968,13 +3964,13 @@
         <v>0.67708333333333337</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -3985,7 +3981,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -3996,7 +3992,7 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -4007,7 +4003,7 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -4018,7 +4014,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -4029,7 +4025,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -4040,7 +4036,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -4051,7 +4047,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -4062,7 +4058,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -4073,7 +4069,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -4084,7 +4080,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -4095,7 +4091,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -4106,7 +4102,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -4130,9 +4126,9 @@
       <selection activeCell="R99" sqref="R99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4164,7 +4160,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" s="3">
         <v>168</v>
       </c>
@@ -4175,7 +4171,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E2" s="3">
         <v>2</v>
@@ -4196,7 +4192,7 @@
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="3">
         <v>212</v>
       </c>
@@ -4204,10 +4200,10 @@
         <v>78</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -4228,7 +4224,7 @@
         <v>0.53472222222222221</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" s="3">
         <v>227</v>
       </c>
@@ -4239,7 +4235,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E4" s="3">
         <v>12</v>
@@ -4260,7 +4256,7 @@
         <v>0.48958333333333331</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" s="3">
         <v>239</v>
       </c>
@@ -4271,7 +4267,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E5" s="3">
         <v>4</v>
@@ -4292,7 +4288,7 @@
         <v>0.55208333333333337</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" s="3">
         <v>271</v>
       </c>
@@ -4300,10 +4296,10 @@
         <v>64</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E6" s="3">
         <v>11</v>
@@ -4324,7 +4320,7 @@
         <v>0.47916666666666669</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" s="3">
         <v>275</v>
       </c>
@@ -4332,10 +4328,10 @@
         <v>67</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E7" s="3">
         <v>6</v>
@@ -4356,7 +4352,7 @@
         <v>0.53472222222222221</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" s="3">
         <v>279</v>
       </c>
@@ -4367,7 +4363,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E8" s="3">
         <v>13</v>
@@ -4388,7 +4384,7 @@
         <v>0.55555555555555558</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" s="3">
         <v>333</v>
       </c>
@@ -4396,10 +4392,10 @@
         <v>79</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E9" s="3">
         <v>9</v>
@@ -4420,7 +4416,7 @@
         <v>0.52083333333333337</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="A10" s="3">
         <v>418</v>
       </c>
@@ -4431,7 +4427,7 @@
         <v>10</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E10" s="3">
         <v>9</v>
@@ -4452,7 +4448,7 @@
         <v>0.52083333333333337</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" s="3">
         <v>481</v>
       </c>
@@ -4463,7 +4459,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E11" s="3">
         <v>4</v>
@@ -4484,7 +4480,7 @@
         <v>0.52083333333333337</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" s="3">
         <v>556</v>
       </c>
@@ -4492,10 +4488,10 @@
         <v>69</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E12" s="3">
         <v>12</v>
@@ -4516,7 +4512,7 @@
         <v>0.51041666666666663</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13" s="3">
         <v>607</v>
       </c>
@@ -4524,10 +4520,10 @@
         <v>77</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E13" s="3">
         <v>9</v>
@@ -4548,7 +4544,7 @@
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" s="3">
         <v>656</v>
       </c>
@@ -4559,7 +4555,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E14" s="3">
         <v>3</v>
@@ -4580,7 +4576,7 @@
         <v>0.50694444444444442</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" s="3">
         <v>661</v>
       </c>
@@ -4588,10 +4584,10 @@
         <v>59</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E15" s="3">
         <v>11</v>
@@ -4612,7 +4608,7 @@
         <v>0.40972222222222221</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" s="3">
         <v>738</v>
       </c>
@@ -4620,10 +4616,10 @@
         <v>69</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E16" s="3">
         <v>1</v>
@@ -4644,7 +4640,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10">
       <c r="A17" s="3">
         <v>775</v>
       </c>
@@ -4652,10 +4648,10 @@
         <v>74</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E17" s="3">
         <v>7</v>
@@ -4676,7 +4672,7 @@
         <v>0.56944444444444442</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10">
       <c r="A18" s="3">
         <v>816</v>
       </c>
@@ -4684,10 +4680,10 @@
         <v>68</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E18" s="3">
         <v>4</v>
@@ -4708,7 +4704,7 @@
         <v>0.52083333333333337</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10">
       <c r="A19" s="3">
         <v>923</v>
       </c>
@@ -4716,10 +4712,10 @@
         <v>63</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E19" s="3">
         <v>7</v>
@@ -4740,7 +4736,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10">
       <c r="A20" s="3">
         <v>963</v>
       </c>
@@ -4751,7 +4747,7 @@
         <v>10</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E20" s="3">
         <v>8</v>
@@ -4772,7 +4768,7 @@
         <v>0.47916666666666669</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10">
       <c r="A21" s="3">
         <v>983</v>
       </c>
@@ -4783,7 +4779,7 @@
         <v>10</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E21" s="3">
         <v>10</v>
@@ -4804,7 +4800,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10">
       <c r="A22" s="3">
         <v>274</v>
       </c>
@@ -4812,10 +4808,10 @@
         <v>56</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E22" s="3">
         <v>7</v>
@@ -4836,7 +4832,7 @@
         <v>0.59722222222222221</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10">
       <c r="A23" s="3">
         <v>285</v>
       </c>
@@ -4847,7 +4843,7 @@
         <v>10</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E23" s="3">
         <v>4</v>
@@ -4868,7 +4864,7 @@
         <v>0.4236111111111111</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10">
       <c r="A24" s="3">
         <v>317</v>
       </c>
@@ -4879,7 +4875,7 @@
         <v>10</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E24" s="3">
         <v>7</v>
@@ -4900,7 +4896,7 @@
         <v>0.61458333333333337</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10">
       <c r="A25" s="3">
         <v>334</v>
       </c>
@@ -4911,7 +4907,7 @@
         <v>10</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E25" s="3">
         <v>6</v>
@@ -4932,7 +4928,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10">
       <c r="A26" s="3">
         <v>380</v>
       </c>
@@ -4940,10 +4936,10 @@
         <v>73</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E26" s="3">
         <v>8</v>
@@ -4964,7 +4960,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10">
       <c r="A27" s="3">
         <v>393</v>
       </c>
@@ -4972,10 +4968,10 @@
         <v>69</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E27" s="3">
         <v>17</v>
@@ -4996,7 +4992,7 @@
         <v>0.47916666666666669</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10">
       <c r="A28" s="3">
         <v>406</v>
       </c>
@@ -5004,10 +5000,10 @@
         <v>62</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E28" s="3">
         <v>11</v>
@@ -5028,7 +5024,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10">
       <c r="A29" s="3">
         <v>445</v>
       </c>
@@ -5039,7 +5035,7 @@
         <v>10</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E29" s="3">
         <v>14</v>
@@ -5060,7 +5056,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10">
       <c r="A30" s="3">
         <v>535</v>
       </c>
@@ -5071,7 +5067,7 @@
         <v>10</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E30" s="3">
         <v>11</v>
@@ -5092,7 +5088,7 @@
         <v>0.47916666666666669</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10">
       <c r="A31" s="3">
         <v>595</v>
       </c>
@@ -5103,7 +5099,7 @@
         <v>10</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E31" s="3">
         <v>8</v>
@@ -5124,7 +5120,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10">
       <c r="A32" s="3">
         <v>633</v>
       </c>
@@ -5132,10 +5128,10 @@
         <v>61</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E32" s="3">
         <v>12</v>
@@ -5156,7 +5152,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10">
       <c r="A33" s="3">
         <v>659</v>
       </c>
@@ -5167,7 +5163,7 @@
         <v>10</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E33" s="3">
         <v>14</v>
@@ -5188,7 +5184,7 @@
         <v>0.46875</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10">
       <c r="A34" s="3">
         <v>717</v>
       </c>
@@ -5199,7 +5195,7 @@
         <v>10</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E34" s="3">
         <v>11</v>
@@ -5220,7 +5216,7 @@
         <v>0.44791666666666669</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10">
       <c r="A35" s="3">
         <v>730</v>
       </c>
@@ -5228,10 +5224,10 @@
         <v>70</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E35" s="3">
         <v>3</v>
@@ -5252,7 +5248,7 @@
         <v>0.40625</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10">
       <c r="A36" s="3">
         <v>739</v>
       </c>
@@ -5263,7 +5259,7 @@
         <v>10</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E36" s="3">
         <v>3</v>
@@ -5284,7 +5280,7 @@
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10">
       <c r="A37" s="3">
         <v>753</v>
       </c>
@@ -5292,10 +5288,10 @@
         <v>67</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E37" s="3">
         <v>6</v>
@@ -5316,7 +5312,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10">
       <c r="A38" s="3">
         <v>787</v>
       </c>
@@ -5324,10 +5320,10 @@
         <v>61</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E38" s="3">
         <v>6</v>
@@ -5348,7 +5344,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10">
       <c r="A39" s="3">
         <v>839</v>
       </c>
@@ -5356,10 +5352,10 @@
         <v>55</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E39" s="3">
         <v>3</v>
@@ -5380,7 +5376,7 @@
         <v>0.51041666666666663</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10">
       <c r="A40" s="3">
         <v>862</v>
       </c>
@@ -5388,10 +5384,10 @@
         <v>57</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E40" s="3">
         <v>3</v>
@@ -5412,7 +5408,7 @@
         <v>0.47916666666666669</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10">
       <c r="A41" s="3">
         <v>888</v>
       </c>
@@ -5423,7 +5419,7 @@
         <v>10</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E41" s="3">
         <v>12</v>
@@ -5444,7 +5440,7 @@
         <v>0.40277777777777779</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10">
       <c r="A42" s="3">
         <v>897</v>
       </c>
@@ -5452,10 +5448,10 @@
         <v>53</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E42" s="3">
         <v>4</v>
@@ -5476,7 +5472,7 @@
         <v>0.60416666666666663</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10">
       <c r="A43" s="3">
         <v>976</v>
       </c>
@@ -5487,7 +5483,7 @@
         <v>10</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E43" s="3">
         <v>5</v>
@@ -5508,7 +5504,7 @@
         <v>0.59722222222222221</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10">
       <c r="A44" s="3">
         <v>111</v>
       </c>
@@ -5519,7 +5515,7 @@
         <v>10</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E44" s="3">
         <v>12</v>
@@ -5532,7 +5528,7 @@
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10">
       <c r="A45" s="3">
         <v>115</v>
       </c>
@@ -5543,7 +5539,7 @@
         <v>10</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E45" s="3">
         <v>11</v>
@@ -5556,7 +5552,7 @@
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10">
       <c r="A46" s="3">
         <v>117</v>
       </c>
@@ -5567,7 +5563,7 @@
         <v>10</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E46" s="3">
         <v>8</v>
@@ -5580,7 +5576,7 @@
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10">
       <c r="A47" s="3">
         <v>234</v>
       </c>
@@ -5591,7 +5587,7 @@
         <v>10</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E47" s="3">
         <v>12</v>
@@ -5604,7 +5600,7 @@
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10">
       <c r="A48" s="3">
         <v>250</v>
       </c>
@@ -5612,10 +5608,10 @@
         <v>72</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E48" s="3">
         <v>11</v>
@@ -5628,7 +5624,7 @@
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10">
       <c r="A49" s="3">
         <v>256</v>
       </c>
@@ -5639,7 +5635,7 @@
         <v>10</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E49" s="3">
         <v>5</v>
@@ -5652,7 +5648,7 @@
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10">
       <c r="A50" s="3">
         <v>353</v>
       </c>
@@ -5660,10 +5656,10 @@
         <v>61</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E50" s="3">
         <v>4</v>
@@ -5676,7 +5672,7 @@
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10">
       <c r="A51" s="3">
         <v>367</v>
       </c>
@@ -5687,7 +5683,7 @@
         <v>10</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E51" s="3">
         <v>3</v>
@@ -5700,7 +5696,7 @@
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10">
       <c r="A52" s="3">
         <v>422</v>
       </c>
@@ -5708,10 +5704,10 @@
         <v>61</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E52" s="3">
         <v>11</v>
@@ -5724,7 +5720,7 @@
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10">
       <c r="A53" s="3">
         <v>427</v>
       </c>
@@ -5732,10 +5728,10 @@
         <v>61</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E53" s="3">
         <v>1</v>
@@ -5748,7 +5744,7 @@
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10">
       <c r="A54" s="3">
         <v>476</v>
       </c>
@@ -5756,10 +5752,10 @@
         <v>77</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E54" s="3">
         <v>10</v>
@@ -5772,7 +5768,7 @@
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10">
       <c r="A55" s="3">
         <v>488</v>
       </c>
@@ -5783,7 +5779,7 @@
         <v>10</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E55" s="3">
         <v>14</v>
@@ -5796,7 +5792,7 @@
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10">
       <c r="A56" s="3">
         <v>495</v>
       </c>
@@ -5807,7 +5803,7 @@
         <v>10</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E56" s="3">
         <v>7</v>
@@ -5820,7 +5816,7 @@
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10">
       <c r="A57" s="3">
         <v>512</v>
       </c>
@@ -5831,7 +5827,7 @@
         <v>10</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E57" s="3">
         <v>9</v>
@@ -5844,7 +5840,7 @@
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10">
       <c r="A58" s="3">
         <v>541</v>
       </c>
@@ -5855,7 +5851,7 @@
         <v>10</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E58" s="3">
         <v>13</v>
@@ -5868,7 +5864,7 @@
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10">
       <c r="A59" s="3">
         <v>553</v>
       </c>
@@ -5879,7 +5875,7 @@
         <v>10</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E59" s="3">
         <v>5</v>
@@ -5892,7 +5888,7 @@
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10">
       <c r="A60" s="3">
         <v>589</v>
       </c>
@@ -5900,10 +5896,10 @@
         <v>72</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E60" s="3">
         <v>3</v>
@@ -5916,7 +5912,7 @@
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10">
       <c r="A61" s="3">
         <v>773</v>
       </c>
@@ -5927,7 +5923,7 @@
         <v>10</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E61" s="3">
         <v>10</v>
@@ -5940,7 +5936,7 @@
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10">
       <c r="A62" s="3">
         <v>859</v>
       </c>
@@ -5951,7 +5947,7 @@
         <v>10</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E62" s="3">
         <v>8</v>
@@ -5964,7 +5960,7 @@
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10">
       <c r="A63" s="3">
         <v>915</v>
       </c>
@@ -5972,10 +5968,10 @@
         <v>54</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E63" s="3">
         <v>5</v>
@@ -5988,7 +5984,7 @@
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10">
       <c r="A64">
         <v>1154</v>
       </c>
@@ -5999,7 +5995,7 @@
         <v>10</v>
       </c>
       <c r="D64" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E64" s="6">
         <v>7</v>
@@ -6011,7 +6007,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10">
       <c r="A65">
         <v>1155</v>
       </c>
@@ -6022,7 +6018,7 @@
         <v>10</v>
       </c>
       <c r="D65" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E65" s="6">
         <v>10</v>
@@ -6034,7 +6030,7 @@
         <v>0.3888888888888889</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10">
       <c r="A66">
         <v>1175</v>
       </c>
@@ -6042,10 +6038,10 @@
         <v>66</v>
       </c>
       <c r="C66" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D66" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E66" s="6">
         <v>5</v>
@@ -6057,7 +6053,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10">
       <c r="A67">
         <v>1194</v>
       </c>
@@ -6065,10 +6061,10 @@
         <v>63</v>
       </c>
       <c r="C67" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D67" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E67" s="6">
         <v>6</v>
@@ -6080,7 +6076,7 @@
         <v>0.4375</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10">
       <c r="A68">
         <v>1196</v>
       </c>
@@ -6091,7 +6087,7 @@
         <v>10</v>
       </c>
       <c r="D68" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E68" s="6">
         <v>12</v>
@@ -6103,7 +6099,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10">
       <c r="A69">
         <v>1214</v>
       </c>
@@ -6111,10 +6107,10 @@
         <v>61</v>
       </c>
       <c r="C69" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D69" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E69" s="6">
         <v>11</v>
@@ -6126,7 +6122,7 @@
         <v>0.52083333333333337</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10">
       <c r="A70">
         <v>1288</v>
       </c>
@@ -6137,7 +6133,7 @@
         <v>10</v>
       </c>
       <c r="D70" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E70" s="6">
         <v>5</v>
@@ -6149,7 +6145,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10">
       <c r="A71">
         <v>1300</v>
       </c>
@@ -6160,7 +6156,7 @@
         <v>10</v>
       </c>
       <c r="D71" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E71" s="6">
         <v>9</v>
@@ -6169,7 +6165,7 @@
         <v>0.47916666666666669</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10">
       <c r="A72">
         <v>1319</v>
       </c>
@@ -6180,7 +6176,7 @@
         <v>10</v>
       </c>
       <c r="D72" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E72" s="6">
         <v>9</v>
@@ -6192,7 +6188,7 @@
         <v>0.6875</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10">
       <c r="A73">
         <v>1325</v>
       </c>
@@ -6200,10 +6196,10 @@
         <v>70</v>
       </c>
       <c r="C73" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D73" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E73" s="6">
         <v>11</v>
@@ -6215,7 +6211,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10">
       <c r="A74">
         <v>1345</v>
       </c>
@@ -6223,10 +6219,10 @@
         <v>69</v>
       </c>
       <c r="C74" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D74" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E74" s="6">
         <v>13</v>
@@ -6238,7 +6234,7 @@
         <v>0.52083333333333337</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10">
       <c r="A75">
         <v>1379</v>
       </c>
@@ -6249,7 +6245,7 @@
         <v>10</v>
       </c>
       <c r="D75" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E75" s="6">
         <v>5</v>
@@ -6261,7 +6257,7 @@
         <v>0.40625</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10">
       <c r="A76">
         <v>1452</v>
       </c>
@@ -6269,10 +6265,10 @@
         <v>71</v>
       </c>
       <c r="C76" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D76" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E76" s="6">
         <v>10</v>
@@ -6284,7 +6280,7 @@
         <v>0.60416666666666663</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10">
       <c r="A77">
         <v>1164</v>
       </c>
@@ -6292,10 +6288,10 @@
         <v>67</v>
       </c>
       <c r="C77" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D77" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E77" s="6">
         <v>11</v>
@@ -6316,7 +6312,7 @@
         <v>0.49305555555555558</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10">
       <c r="A78">
         <v>1176</v>
       </c>
@@ -6327,7 +6323,7 @@
         <v>10</v>
       </c>
       <c r="D78" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E78" s="6">
         <v>13</v>
@@ -6348,7 +6344,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10">
       <c r="A79">
         <v>1266</v>
       </c>
@@ -6356,10 +6352,10 @@
         <v>70</v>
       </c>
       <c r="C79" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D79" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E79" s="6">
         <v>10</v>
@@ -6380,7 +6376,7 @@
         <v>0.49305555555555558</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10">
       <c r="A80">
         <v>1312</v>
       </c>
@@ -6388,10 +6384,10 @@
         <v>71</v>
       </c>
       <c r="C80" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D80" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E80" s="6">
         <v>8</v>
@@ -6412,7 +6408,7 @@
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10">
       <c r="A81">
         <v>1374</v>
       </c>
@@ -6423,7 +6419,7 @@
         <v>10</v>
       </c>
       <c r="D81" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E81" s="6">
         <v>7</v>
@@ -6444,7 +6440,7 @@
         <v>0.67708333333333337</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10">
       <c r="A82">
         <v>1391</v>
       </c>
@@ -6452,10 +6448,10 @@
         <v>69</v>
       </c>
       <c r="C82" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D82" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E82" s="6">
         <v>4</v>
@@ -6476,7 +6472,7 @@
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10">
       <c r="A83">
         <v>1102</v>
       </c>
@@ -6487,7 +6483,7 @@
         <v>10</v>
       </c>
       <c r="D83" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E83" s="6">
         <v>11</v>
@@ -6508,7 +6504,7 @@
         <v>0.37152777777777779</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10">
       <c r="A84">
         <v>1215</v>
       </c>
@@ -6519,7 +6515,7 @@
         <v>10</v>
       </c>
       <c r="D84" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E84" s="6">
         <v>10</v>
@@ -6540,7 +6536,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10">
       <c r="A85">
         <v>1224</v>
       </c>
@@ -6548,10 +6544,10 @@
         <v>69</v>
       </c>
       <c r="C85" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D85" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E85" s="6">
         <v>9</v>
@@ -6572,7 +6568,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10">
       <c r="A86">
         <v>1260</v>
       </c>
@@ -6580,10 +6576,10 @@
         <v>65</v>
       </c>
       <c r="C86" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D86" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E86" s="6">
         <v>9</v>
@@ -6604,7 +6600,7 @@
         <v>0.47916666666666669</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10">
       <c r="A87">
         <v>1326</v>
       </c>
@@ -6612,10 +6608,10 @@
         <v>66</v>
       </c>
       <c r="C87" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D87" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E87" s="6">
         <v>6</v>
@@ -6636,7 +6632,7 @@
         <v>0.52083333333333337</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10">
       <c r="A88">
         <v>1348</v>
       </c>
@@ -6647,7 +6643,7 @@
         <v>10</v>
       </c>
       <c r="D88" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E88" s="6">
         <v>11</v>
@@ -6668,7 +6664,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10">
       <c r="A89">
         <v>1388</v>
       </c>
@@ -6679,7 +6675,7 @@
         <v>10</v>
       </c>
       <c r="D89" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E89" s="6">
         <v>9</v>
@@ -6700,7 +6696,7 @@
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10">
       <c r="A90" s="8">
         <v>1454</v>
       </c>
@@ -6711,7 +6707,7 @@
         <v>10</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E90" s="9">
         <v>12</v>
@@ -6732,7 +6728,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10">
       <c r="A91" s="8">
         <v>1455</v>
       </c>
@@ -6740,10 +6736,10 @@
         <v>68</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D91" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E91" s="9">
         <v>12</v>
@@ -6764,7 +6760,7 @@
         <v>0.72916666666666663</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10">
       <c r="A92" s="8">
         <v>1466</v>
       </c>
@@ -6775,7 +6771,7 @@
         <v>10</v>
       </c>
       <c r="D92" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E92" s="9">
         <v>10</v>
@@ -6788,7 +6784,7 @@
       <c r="I92" s="8"/>
       <c r="J92" s="8"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10">
       <c r="A93" s="8">
         <v>1525</v>
       </c>
@@ -6799,7 +6795,7 @@
         <v>10</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E93" s="9">
         <v>6</v>
@@ -6820,7 +6816,7 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10">
       <c r="A94" s="8">
         <v>1543</v>
       </c>
@@ -6831,7 +6827,7 @@
         <v>10</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E94" s="8">
         <v>10</v>
@@ -6852,7 +6848,7 @@
         <v>0.47916666666666669</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10">
       <c r="A95" s="8">
         <v>1586</v>
       </c>
@@ -6860,10 +6856,10 @@
         <v>71</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E95" s="8">
         <v>14</v>
@@ -6884,7 +6880,7 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10">
       <c r="A96" s="8">
         <v>1590</v>
       </c>
@@ -6892,10 +6888,10 @@
         <v>69</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E96" s="8">
         <v>11</v>
@@ -6916,7 +6912,7 @@
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10">
       <c r="A97" s="8">
         <v>1631</v>
       </c>
@@ -6924,10 +6920,10 @@
         <v>66</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E97" s="8">
         <v>16</v>
@@ -6948,7 +6944,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10">
       <c r="A98" s="8">
         <v>1693</v>
       </c>
@@ -6959,7 +6955,7 @@
         <v>10</v>
       </c>
       <c r="D98" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E98" s="8">
         <v>12</v>
@@ -6980,7 +6976,7 @@
         <v>0.70833333333333337</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10">
       <c r="A99" s="8">
         <v>1720</v>
       </c>
@@ -6988,10 +6984,10 @@
         <v>66</v>
       </c>
       <c r="C99" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D99" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E99" s="8">
         <v>8</v>
@@ -7012,7 +7008,7 @@
         <v>0.35416666666666669</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10">
       <c r="A100" s="8">
         <v>1732</v>
       </c>
@@ -7020,10 +7016,10 @@
         <v>70</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D100" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E100" s="8">
         <v>9</v>
@@ -7044,7 +7040,7 @@
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10">
       <c r="A101">
         <v>1532</v>
       </c>
@@ -7052,10 +7048,10 @@
         <v>72</v>
       </c>
       <c r="C101" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D101" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E101" s="6">
         <v>12</v>
@@ -7067,7 +7063,7 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10">
       <c r="A102">
         <v>1596</v>
       </c>
@@ -7078,7 +7074,7 @@
         <v>10</v>
       </c>
       <c r="D102" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E102">
         <v>16</v>
@@ -7099,7 +7095,7 @@
         <v>0.54861111111111116</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10">
       <c r="A103">
         <v>1663</v>
       </c>
@@ -7110,7 +7106,7 @@
         <v>10</v>
       </c>
       <c r="D103" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E103">
         <v>11</v>
@@ -7131,7 +7127,7 @@
         <v>0.49305555555555558</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10">
       <c r="A104">
         <v>1706</v>
       </c>
@@ -7142,7 +7138,7 @@
         <v>10</v>
       </c>
       <c r="D104" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E104">
         <v>10</v>
@@ -7163,7 +7159,7 @@
         <v>0.40625</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10">
       <c r="A105">
         <v>1722</v>
       </c>
@@ -7174,7 +7170,7 @@
         <v>10</v>
       </c>
       <c r="D105" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E105">
         <v>7</v>

</xml_diff>